<commit_message>
bulk student xlsx import
</commit_message>
<xml_diff>
--- a/daemon/files/student_roster.xlsx
+++ b/daemon/files/student_roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Code\Python\ledscreen\daemon\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D4E34C-1785-4A36-B282-4DF7346CA1FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0F675-8C68-4AC8-B2B2-29CCB47F5A4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>run_privilege</t>
-  </si>
-  <si>
-    <t>max_runtime</t>
-  </si>
-  <si>
-    <t>expiry</t>
-  </si>
-  <si>
-    <t>lock</t>
-  </si>
-  <si>
-    <t>comment</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Run Privilege</t>
+  </si>
+  <si>
+    <t>Max Runtime</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>bbbbbb</t>
+  </si>
+  <si>
+    <t>simulate</t>
+  </si>
+  <si>
+    <t>screen</t>
+  </si>
+  <si>
+    <t>june 1st</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Really cool student</t>
+  </si>
+  <si>
+    <t>Not so cool student</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Thing One</t>
+  </si>
+  <si>
+    <t>Thing Two</t>
   </si>
 </sst>
 </file>
@@ -81,8 +114,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,43 +411,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="5" width="24.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44216</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>